<commit_message>
marked necessary tests for jubula
</commit_message>
<xml_diff>
--- a/Project Assignments/Assignment 1/‏‏G1_Acceptance.Ass1.xlsx
+++ b/Project Assignments/Assignment 1/‏‏G1_Acceptance.Ass1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leehu\Desktop\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\project2\Project Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF44D5B2-F77F-42FD-B1BB-38F0D33DDD49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CBCEEB33-43CF-45A0-956C-B39C2D4E436E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="request submission" sheetId="1" r:id="rId1"/>
@@ -544,7 +543,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -563,12 +562,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -583,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,6 +607,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,59 +939,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6588D779-DA2D-4DE3-9387-6E8C06BB5375}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F22" sqref="A22:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.9140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.08203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.09765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -982,27 +1011,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" ht="184.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="182" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="179.4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1022,27 +1051,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:6" ht="184.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="188.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="188.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1062,87 +1091,87 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="193" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:6" ht="193.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="188.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:6" ht="188.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="168.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:6" ht="168.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="118" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:6" ht="118.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="168" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="165.6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
         <v>27</v>
@@ -1160,58 +1189,59 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="168" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:6" ht="165.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="168" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:6" ht="165.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="7">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the acceptance_test file and finished the jubula assignment
</commit_message>
<xml_diff>
--- a/Project Assignments/Assignment 1/‏‏G1_Acceptance.Ass1.xlsx
+++ b/Project Assignments/Assignment 1/‏‏G1_Acceptance.Ass1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="request submission" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Comments</t>
   </si>
@@ -338,35 +338,6 @@
     <t>RequestSubmissionEmptyFailed</t>
   </si>
   <si>
-    <r>
-      <t>Open the change request page:
-1.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Leave all the fields empty</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="177"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2. Click "Submit" button</t>
-    </r>
-  </si>
-  <si>
     <t>The system throws out 
 a warning message "Must fill all the required fields"
 All required fields are marked in red</t>
@@ -539,12 +510,43 @@
   <si>
     <t>עידו קדוש - Idokadosh1@gmail.com</t>
   </si>
+  <si>
+    <r>
+      <t>Open the change request page:
+1.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leave all the fields empty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Click "Submit" button</t>
+    </r>
+  </si>
+  <si>
+    <t>disabled on our project</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,8 +563,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +598,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -594,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -625,6 +648,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="A22:F22"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F13" sqref="C13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -953,45 +991,47 @@
     <col min="3" max="3" width="23.09765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="6" max="6" width="9" style="1"/>
+    <col min="7" max="7" width="19.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,163 +1051,167 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="184.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:7" ht="184.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="179.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:7" ht="179.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="184.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="184.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="188.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" ht="188.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="193.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="G14" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="193.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="188.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:7" ht="188.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="11">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="168.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="E17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="11">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="118.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1177,33 +1221,33 @@
         <v>27</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="165.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="6">
+      <c r="E20" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="10">
         <v>10</v>
       </c>
     </row>
@@ -1213,35 +1257,35 @@
         <v>27</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="8">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="A22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="C22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="7">
+      <c r="E22" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="15">
         <v>12</v>
       </c>
     </row>

</xml_diff>